<commit_message>
New matrix for added node
</commit_message>
<xml_diff>
--- a/Add Node System Change.xlsx
+++ b/Add Node System Change.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samue\Documents\GitHub\capitalbikeshare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B7717E-890C-4683-A2F1-104696CAF849}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51926993-31AC-4082-B5FB-525890A09E21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{555ADB72-8A8C-4859-AADA-6BBB5665AFD2}"/>
+    <workbookView xWindow="672" yWindow="306" windowWidth="17334" windowHeight="12162" xr2:uid="{555ADB72-8A8C-4859-AADA-6BBB5665AFD2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>cells</t>
   </si>
@@ -58,12 +58,49 @@
   </si>
   <si>
     <t>New</t>
+  </si>
+  <si>
+    <t>Change</t>
+  </si>
+  <si>
+    <t>Rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New </t>
+  </si>
+  <si>
+    <t>Fraction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Base </t>
+  </si>
+  <si>
+    <t>Base</t>
+  </si>
+  <si>
+    <t>Occur</t>
+  </si>
+  <si>
+    <t>Modified</t>
+  </si>
+  <si>
+    <t>Geography</t>
+  </si>
+  <si>
+    <t>System</t>
+  </si>
+  <si>
+    <t>Station</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="168" formatCode="0.0%"/>
+    <numFmt numFmtId="172" formatCode="0.00000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -109,7 +146,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -117,12 +154,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -146,15 +186,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>57151</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>102871</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>594361</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>802</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>160822</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -177,7 +217,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="57151" y="2415540"/>
+          <a:off x="102871" y="3124200"/>
           <a:ext cx="3737610" cy="3803182"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -190,15 +230,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>83820</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>160021</xdr:rowOff>
+      <xdr:colOff>186690</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>133351</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>71208</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>76201</xdr:rowOff>
+      <xdr:colOff>288378</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>49531</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -221,7 +261,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3924300" y="2354581"/>
+          <a:off x="4027170" y="3059431"/>
           <a:ext cx="3827868" cy="3939540"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -531,15 +571,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17A6C4E1-D05B-4191-9D6A-E26E00ED9E8A}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4:M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="7" max="7" width="5.62890625" customWidth="1"/>
+    <col min="10" max="10" width="10.47265625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A1">
         <v>10000</v>
       </c>
@@ -547,25 +591,58 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4" s="4" t="s">
+      <c r="J3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -575,12 +652,34 @@
       <c r="C5" s="2">
         <v>3975</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="5">
         <f>(C5-B5)/B5</f>
         <v>-0.12290379523389232</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E5" s="4"/>
+      <c r="F5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -592,27 +691,47 @@
         <f>SUM(C7:C13)</f>
         <v>6025</v>
       </c>
-      <c r="D6" s="3">
-        <f t="shared" ref="D6:D13" si="0">(C6-B6)/B6</f>
+      <c r="D6" s="5">
+        <f t="shared" ref="D6:D12" si="0">(C6-B6)/B6</f>
         <v>0.10186539868324798</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="J6" s="7"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1">
-        <v>31113</v>
+        <v>10000</v>
       </c>
       <c r="B7" s="2">
-        <v>628</v>
+        <v>0</v>
       </c>
       <c r="C7" s="2">
-        <v>235</v>
-      </c>
-      <c r="D7" s="3">
-        <f t="shared" si="0"/>
-        <v>-0.62579617834394907</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>1387</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>27</v>
+      </c>
+      <c r="I7" s="6"/>
+      <c r="J7" s="7"/>
+      <c r="K7">
+        <f>G7*(1+D6)</f>
+        <v>29.750365764447697</v>
+      </c>
+      <c r="L7">
+        <f>1-SUM(L8:L13)</f>
+        <v>0.20376574214154375</v>
+      </c>
+      <c r="M7" s="1">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1">
         <v>31104</v>
       </c>
@@ -622,86 +741,264 @@
       <c r="C8" s="2">
         <v>530</v>
       </c>
-      <c r="D8" s="3">
-        <f t="shared" si="0"/>
+      <c r="D8" s="5">
+        <f>(C8-B8)/B8</f>
         <v>-3.4608378870673952E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="F8">
+        <v>0.18627199999999999</v>
+      </c>
+      <c r="G8">
+        <v>27</v>
+      </c>
+      <c r="H8">
+        <f>F8*G8</f>
+        <v>5.029344</v>
+      </c>
+      <c r="I8" s="6">
+        <f t="shared" ref="I8:I13" si="1">D8</f>
+        <v>-3.4608378870673952E-2</v>
+      </c>
+      <c r="J8" s="7">
+        <f>H8*(1+I8)</f>
+        <v>4.8552865573770498</v>
+      </c>
+      <c r="K8">
+        <f>K7</f>
+        <v>29.750365764447697</v>
+      </c>
+      <c r="L8">
+        <f>J8/K8</f>
+        <v>0.16320090300130757</v>
+      </c>
+      <c r="M8" s="1">
+        <v>31104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1">
+        <v>31110</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1639</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1221</v>
+      </c>
+      <c r="D9" s="5">
+        <f>(C9-B9)/B9</f>
+        <v>-0.25503355704697989</v>
+      </c>
+      <c r="F9">
+        <v>0.25479400000000002</v>
+      </c>
+      <c r="G9">
+        <v>27</v>
+      </c>
+      <c r="H9">
+        <f t="shared" ref="H9:H13" si="2">F9*G9</f>
+        <v>6.8794380000000004</v>
+      </c>
+      <c r="I9" s="6">
+        <f t="shared" si="1"/>
+        <v>-0.25503355704697989</v>
+      </c>
+      <c r="J9" s="7">
+        <f t="shared" ref="J9:J13" si="3">H9*(1+I9)</f>
+        <v>5.1249504563758386</v>
+      </c>
+      <c r="K9">
+        <f t="shared" ref="K9:K13" si="4">K8</f>
+        <v>29.750365764447697</v>
+      </c>
+      <c r="L9">
+        <f t="shared" ref="L9:L13" si="5">J9/K9</f>
+        <v>0.17226512429975771</v>
+      </c>
+      <c r="M9" s="1">
+        <v>31110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="1">
+        <v>31113</v>
+      </c>
+      <c r="B10" s="2">
+        <v>628</v>
+      </c>
+      <c r="C10" s="2">
+        <v>235</v>
+      </c>
+      <c r="D10" s="5">
+        <f>(C10-B10)/B10</f>
+        <v>-0.62579617834394907</v>
+      </c>
+      <c r="F10">
+        <v>8.1865999999999994E-2</v>
+      </c>
+      <c r="G10">
+        <v>27</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="2"/>
+        <v>2.2103820000000001</v>
+      </c>
+      <c r="I10" s="6">
+        <f t="shared" si="1"/>
+        <v>-0.62579617834394907</v>
+      </c>
+      <c r="J10" s="7">
+        <f t="shared" si="3"/>
+        <v>0.8271333917197452</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="4"/>
+        <v>29.750365764447697</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="5"/>
+        <v>2.7802461262785103E-2</v>
+      </c>
+      <c r="M10" s="1">
+        <v>31113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="1">
+        <v>31114</v>
+      </c>
+      <c r="B11" s="2">
+        <v>189</v>
+      </c>
+      <c r="C11" s="2">
+        <v>189</v>
+      </c>
+      <c r="D11" s="5">
+        <f>(C11-B11)/B11</f>
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0.17749599999999999</v>
+      </c>
+      <c r="G11">
+        <v>27</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="2"/>
+        <v>4.7923919999999995</v>
+      </c>
+      <c r="I11" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="7">
+        <f t="shared" si="3"/>
+        <v>4.7923919999999995</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="4"/>
+        <v>29.750365764447697</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="5"/>
+        <v>0.16108682622406637</v>
+      </c>
+      <c r="M11" s="1">
+        <v>31114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="1">
+        <v>31116</v>
+      </c>
+      <c r="B12" s="2">
+        <v>986</v>
+      </c>
+      <c r="C12" s="2">
+        <v>986</v>
+      </c>
+      <c r="D12" s="5">
+        <f>(C12-B12)/B12</f>
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0.16950200000000001</v>
+      </c>
+      <c r="G12">
+        <v>27</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="2"/>
+        <v>4.5765540000000007</v>
+      </c>
+      <c r="I12" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="7">
+        <f t="shared" si="3"/>
+        <v>4.5765540000000007</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="4"/>
+        <v>29.750365764447697</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="5"/>
+        <v>0.15383185659751039</v>
+      </c>
+      <c r="M12" s="1">
+        <v>31116</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="1">
         <v>31296</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B13" s="2">
         <v>1477</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C13" s="2">
         <v>1477</v>
       </c>
-      <c r="D9" s="3">
-        <f t="shared" si="0"/>
+      <c r="D13" s="5">
+        <f>(C13-B13)/B13</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="1">
-        <v>31114</v>
-      </c>
-      <c r="B10" s="2">
-        <v>189</v>
-      </c>
-      <c r="C10" s="2">
-        <v>189</v>
-      </c>
-      <c r="D10" s="3">
-        <f t="shared" si="0"/>
+      <c r="F13">
+        <v>0.13007199999999999</v>
+      </c>
+      <c r="G13">
+        <v>27</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="2"/>
+        <v>3.5119439999999997</v>
+      </c>
+      <c r="I13" s="6">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="1">
-        <v>31116</v>
-      </c>
-      <c r="B11" s="2">
-        <v>986</v>
-      </c>
-      <c r="C11" s="2">
-        <v>986</v>
-      </c>
-      <c r="D11" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="1">
-        <v>31110</v>
-      </c>
-      <c r="B12" s="2">
-        <v>1639</v>
-      </c>
-      <c r="C12" s="2">
-        <v>1221</v>
-      </c>
-      <c r="D12" s="3">
-        <f t="shared" si="0"/>
-        <v>-0.25503355704697989</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="1">
-        <v>1000</v>
-      </c>
-      <c r="B13" s="2">
-        <v>0</v>
-      </c>
-      <c r="C13" s="2">
-        <v>1387</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>5</v>
+      <c r="J13" s="7">
+        <f t="shared" si="3"/>
+        <v>3.5119439999999997</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="4"/>
+        <v>29.750365764447697</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="5"/>
+        <v>0.11804708647302903</v>
+      </c>
+      <c r="M13" s="1">
+        <v>31296</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:D13">
+    <sortCondition ref="A7:A13"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
Update Add Node System Change.xlsx
</commit_message>
<xml_diff>
--- a/Add Node System Change.xlsx
+++ b/Add Node System Change.xlsx
@@ -8,13 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samue\Documents\GitHub\capitalbikeshare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51926993-31AC-4082-B5FB-525890A09E21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C6D68E6-EF8D-4FAD-8AF8-192F5BDD3245}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="672" yWindow="306" windowWidth="17334" windowHeight="12162" xr2:uid="{555ADB72-8A8C-4859-AADA-6BBB5665AFD2}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" activeTab="1" xr2:uid="{555ADB72-8A8C-4859-AADA-6BBB5665AFD2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Geographic Change" sheetId="1" r:id="rId1"/>
+    <sheet name="JointDistribution" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="change31104">JointDistribution!$D$28</definedName>
+    <definedName name="change31110">JointDistribution!$D$29</definedName>
+    <definedName name="change31113">JointDistribution!$D$30</definedName>
+    <definedName name="change31114">JointDistribution!$D$30</definedName>
+    <definedName name="N_A" comment="change31104">JointDistribution!$D$28</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
   <si>
     <t>cells</t>
   </si>
@@ -91,6 +99,18 @@
   </si>
   <si>
     <t>Station</t>
+  </si>
+  <si>
+    <t>From \ To</t>
+  </si>
+  <si>
+    <t>sum</t>
+  </si>
+  <si>
+    <t>Original</t>
+  </si>
+  <si>
+    <t>Proposed</t>
   </si>
 </sst>
 </file>
@@ -98,8 +118,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="0.0%"/>
-    <numFmt numFmtId="172" formatCode="0.00000"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -158,10 +178,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -267,6 +287,163 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1025" name="AutoShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38DEF345-6747-43B4-B53F-6C77BA900635}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10126980" y="731520"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1026" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBC04B66-FF1A-4466-B890-5BA98394DC26}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9486900" y="1097280"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>384809</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>11430</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>18998</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65F05E34-787A-4E35-9F16-1DACD443D43F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9231629" y="925830"/>
+          <a:ext cx="4114749" cy="2884170"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -571,10 +748,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17A6C4E1-D05B-4191-9D6A-E26E00ED9E8A}">
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4:M13"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -692,7 +869,7 @@
         <v>6025</v>
       </c>
       <c r="D6" s="5">
-        <f t="shared" ref="D6:D12" si="0">(C6-B6)/B6</f>
+        <f t="shared" ref="D6" si="0">(C6-B6)/B6</f>
         <v>0.10186539868324798</v>
       </c>
       <c r="E6" s="4"/>
@@ -725,7 +902,7 @@
       </c>
       <c r="L7">
         <f>1-SUM(L8:L13)</f>
-        <v>0.20376574214154375</v>
+        <v>0.22088494431805294</v>
       </c>
       <c r="M7" s="1">
         <v>10000</v>
@@ -742,26 +919,26 @@
         <v>530</v>
       </c>
       <c r="D8" s="5">
-        <f>(C8-B8)/B8</f>
+        <f t="shared" ref="D8:D13" si="1">(C8-B8)/B8</f>
         <v>-3.4608378870673952E-2</v>
       </c>
       <c r="F8">
-        <v>0.18627199999999999</v>
+        <v>0.17585100000000001</v>
       </c>
       <c r="G8">
         <v>27</v>
       </c>
       <c r="H8">
         <f>F8*G8</f>
-        <v>5.029344</v>
+        <v>4.7479770000000006</v>
       </c>
       <c r="I8" s="6">
-        <f t="shared" ref="I8:I13" si="1">D8</f>
+        <f t="shared" ref="I8:I13" si="2">D8</f>
         <v>-3.4608378870673952E-2</v>
       </c>
       <c r="J8" s="7">
         <f>H8*(1+I8)</f>
-        <v>4.8552865573770498</v>
+        <v>4.5836572131147548</v>
       </c>
       <c r="K8">
         <f>K7</f>
@@ -769,7 +946,7 @@
       </c>
       <c r="L8">
         <f>J8/K8</f>
-        <v>0.16320090300130757</v>
+        <v>0.15407061712808653</v>
       </c>
       <c r="M8" s="1">
         <v>31104</v>
@@ -786,34 +963,34 @@
         <v>1221</v>
       </c>
       <c r="D9" s="5">
-        <f>(C9-B9)/B9</f>
+        <f t="shared" si="1"/>
         <v>-0.25503355704697989</v>
       </c>
       <c r="F9">
-        <v>0.25479400000000002</v>
+        <v>0.22320699999999999</v>
       </c>
       <c r="G9">
         <v>27</v>
       </c>
       <c r="H9">
-        <f t="shared" ref="H9:H13" si="2">F9*G9</f>
-        <v>6.8794380000000004</v>
+        <f t="shared" ref="H9:H13" si="3">F9*G9</f>
+        <v>6.0265889999999995</v>
       </c>
       <c r="I9" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.25503355704697989</v>
       </c>
       <c r="J9" s="7">
-        <f t="shared" ref="J9:J13" si="3">H9*(1+I9)</f>
-        <v>5.1249504563758386</v>
+        <f t="shared" ref="J9:J13" si="4">H9*(1+I9)</f>
+        <v>4.4896065704697978</v>
       </c>
       <c r="K9">
-        <f t="shared" ref="K9:K13" si="4">K8</f>
+        <f t="shared" ref="K9:K13" si="5">K8</f>
         <v>29.750365764447697</v>
       </c>
       <c r="L9">
-        <f t="shared" ref="L9:L13" si="5">J9/K9</f>
-        <v>0.17226512429975771</v>
+        <f t="shared" ref="L9:L13" si="6">J9/K9</f>
+        <v>0.15090928985602492</v>
       </c>
       <c r="M9" s="1">
         <v>31110</v>
@@ -830,34 +1007,34 @@
         <v>235</v>
       </c>
       <c r="D10" s="5">
-        <f>(C10-B10)/B10</f>
+        <f t="shared" si="1"/>
         <v>-0.62579617834394907</v>
       </c>
       <c r="F10">
-        <v>8.1865999999999994E-2</v>
+        <v>0.12545600000000001</v>
       </c>
       <c r="G10">
         <v>27</v>
       </c>
       <c r="H10">
+        <f t="shared" si="3"/>
+        <v>3.3873120000000005</v>
+      </c>
+      <c r="I10" s="6">
         <f t="shared" si="2"/>
-        <v>2.2103820000000001</v>
-      </c>
-      <c r="I10" s="6">
-        <f t="shared" si="1"/>
         <v>-0.62579617834394907</v>
       </c>
       <c r="J10" s="7">
-        <f t="shared" si="3"/>
-        <v>0.8271333917197452</v>
+        <f t="shared" si="4"/>
+        <v>1.2675450955414014</v>
       </c>
       <c r="K10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>29.750365764447697</v>
       </c>
       <c r="L10">
-        <f t="shared" si="5"/>
-        <v>2.7802461262785103E-2</v>
+        <f t="shared" si="6"/>
+        <v>4.2606034009038771E-2</v>
       </c>
       <c r="M10" s="1">
         <v>31113</v>
@@ -874,34 +1051,34 @@
         <v>189</v>
       </c>
       <c r="D11" s="5">
-        <f>(C11-B11)/B11</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F11">
-        <v>0.17749599999999999</v>
+        <v>0.18324599999999999</v>
       </c>
       <c r="G11">
         <v>27</v>
       </c>
       <c r="H11">
+        <f t="shared" si="3"/>
+        <v>4.9476420000000001</v>
+      </c>
+      <c r="I11" s="6">
         <f t="shared" si="2"/>
-        <v>4.7923919999999995</v>
-      </c>
-      <c r="I11" s="6">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J11" s="7">
-        <f t="shared" si="3"/>
-        <v>4.7923919999999995</v>
+        <f t="shared" si="4"/>
+        <v>4.9476420000000001</v>
       </c>
       <c r="K11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>29.750365764447697</v>
       </c>
       <c r="L11">
-        <f t="shared" si="5"/>
-        <v>0.16108682622406637</v>
+        <f t="shared" si="6"/>
+        <v>0.16630524946058092</v>
       </c>
       <c r="M11" s="1">
         <v>31114</v>
@@ -918,34 +1095,34 @@
         <v>986</v>
       </c>
       <c r="D12" s="5">
-        <f>(C12-B12)/B12</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F12">
-        <v>0.16950200000000001</v>
+        <v>0.131635</v>
       </c>
       <c r="G12">
         <v>27</v>
       </c>
       <c r="H12">
+        <f t="shared" si="3"/>
+        <v>3.5541450000000001</v>
+      </c>
+      <c r="I12" s="6">
         <f t="shared" si="2"/>
-        <v>4.5765540000000007</v>
-      </c>
-      <c r="I12" s="6">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J12" s="7">
-        <f t="shared" si="3"/>
-        <v>4.5765540000000007</v>
+        <f t="shared" si="4"/>
+        <v>3.5541450000000001</v>
       </c>
       <c r="K12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>29.750365764447697</v>
       </c>
       <c r="L12">
-        <f t="shared" si="5"/>
-        <v>0.15383185659751039</v>
+        <f t="shared" si="6"/>
+        <v>0.11946559004149378</v>
       </c>
       <c r="M12" s="1">
         <v>31116</v>
@@ -962,37 +1139,47 @@
         <v>1477</v>
       </c>
       <c r="D13" s="5">
-        <f>(C13-B13)/B13</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F13">
-        <v>0.13007199999999999</v>
+        <v>0.160606</v>
       </c>
       <c r="G13">
         <v>27</v>
       </c>
       <c r="H13">
+        <f t="shared" si="3"/>
+        <v>4.3363620000000003</v>
+      </c>
+      <c r="I13" s="6">
         <f t="shared" si="2"/>
-        <v>3.5119439999999997</v>
-      </c>
-      <c r="I13" s="6">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J13" s="7">
-        <f t="shared" si="3"/>
-        <v>3.5119439999999997</v>
+        <f t="shared" si="4"/>
+        <v>4.3363620000000003</v>
       </c>
       <c r="K13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>29.750365764447697</v>
       </c>
       <c r="L13">
-        <f t="shared" si="5"/>
-        <v>0.11804708647302903</v>
+        <f t="shared" si="6"/>
+        <v>0.14575827518672199</v>
       </c>
       <c r="M13" s="1">
         <v>31296</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="F14">
+        <f>SUM(F7:F13)</f>
+        <v>1.0000010000000001</v>
+      </c>
+      <c r="L14">
+        <f>SUM(L7:L13)</f>
+        <v>0.99999999999999989</v>
       </c>
     </row>
   </sheetData>
@@ -1003,4 +1190,755 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8996F70-2DF4-4A14-99FE-06439C1F33BD}">
+  <dimension ref="A2:O33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15:L20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="5" max="5" width="8.83984375" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="E2" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="4">
+        <v>31104</v>
+      </c>
+      <c r="G3" s="4">
+        <v>31110</v>
+      </c>
+      <c r="H3" s="4">
+        <v>31113</v>
+      </c>
+      <c r="I3" s="4">
+        <v>31114</v>
+      </c>
+      <c r="J3" s="4">
+        <v>31116</v>
+      </c>
+      <c r="K3" s="4">
+        <v>31296</v>
+      </c>
+      <c r="L3" s="4">
+        <v>10000</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="4">
+        <v>31104</v>
+      </c>
+      <c r="F4">
+        <v>8.9562000000000003E-2</v>
+      </c>
+      <c r="G4">
+        <v>0.25373200000000001</v>
+      </c>
+      <c r="H4">
+        <v>8.9552000000000007E-2</v>
+      </c>
+      <c r="I4">
+        <v>0.19900499999999999</v>
+      </c>
+      <c r="J4">
+        <v>0.23383100000000001</v>
+      </c>
+      <c r="K4">
+        <v>0.134328</v>
+      </c>
+      <c r="L4"/>
+      <c r="M4">
+        <f>SUM(F4:K4)</f>
+        <v>1.0000100000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="E5" s="4">
+        <v>31110</v>
+      </c>
+      <c r="F5">
+        <v>0.14285700000000001</v>
+      </c>
+      <c r="G5">
+        <v>0.13364100000000001</v>
+      </c>
+      <c r="H5">
+        <v>8.2948999999999995E-2</v>
+      </c>
+      <c r="I5">
+        <v>0.26728099999999999</v>
+      </c>
+      <c r="J5">
+        <v>0.11981600000000001</v>
+      </c>
+      <c r="K5">
+        <v>0.25345600000000001</v>
+      </c>
+      <c r="M5">
+        <f t="shared" ref="M5:M9" si="0">SUM(F5:K5)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6">
+        <v>0.22088494431805294</v>
+      </c>
+      <c r="B6">
+        <v>10000</v>
+      </c>
+      <c r="E6" s="4">
+        <v>31113</v>
+      </c>
+      <c r="F6">
+        <v>6.6986000000000004E-2</v>
+      </c>
+      <c r="G6">
+        <v>0.32057400000000003</v>
+      </c>
+      <c r="H6">
+        <v>0.100478</v>
+      </c>
+      <c r="I6">
+        <v>0.15789500000000001</v>
+      </c>
+      <c r="J6">
+        <v>0.143541</v>
+      </c>
+      <c r="K6">
+        <v>0.21052599999999999</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7">
+        <v>0.15407061712808653</v>
+      </c>
+      <c r="B7">
+        <v>31104</v>
+      </c>
+      <c r="E7" s="4">
+        <v>31114</v>
+      </c>
+      <c r="F7">
+        <v>0.20535700000000001</v>
+      </c>
+      <c r="G7">
+        <v>0.37946400000000002</v>
+      </c>
+      <c r="H7">
+        <v>4.9106999999999998E-2</v>
+      </c>
+      <c r="I7">
+        <v>0.10267900000000001</v>
+      </c>
+      <c r="J7">
+        <v>4.4643000000000002E-2</v>
+      </c>
+      <c r="K7">
+        <v>0.21875</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8">
+        <v>0.15090928985602492</v>
+      </c>
+      <c r="B8">
+        <v>31110</v>
+      </c>
+      <c r="E8" s="4">
+        <v>31116</v>
+      </c>
+      <c r="F8">
+        <v>0.23188400000000001</v>
+      </c>
+      <c r="G8">
+        <v>0.23913000000000001</v>
+      </c>
+      <c r="H8">
+        <v>0.108696</v>
+      </c>
+      <c r="I8">
+        <v>0.101449</v>
+      </c>
+      <c r="J8">
+        <v>8.6957000000000007E-2</v>
+      </c>
+      <c r="K8">
+        <v>0.23188400000000001</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9">
+        <v>4.2606034009038771E-2</v>
+      </c>
+      <c r="B9">
+        <v>31113</v>
+      </c>
+      <c r="E9" s="4">
+        <v>31296</v>
+      </c>
+      <c r="F9">
+        <v>0.11788700000000001</v>
+      </c>
+      <c r="G9">
+        <v>0.26441999999999999</v>
+      </c>
+      <c r="H9">
+        <v>0.191057</v>
+      </c>
+      <c r="I9">
+        <v>0.18699199999999999</v>
+      </c>
+      <c r="J9">
+        <v>0.138211</v>
+      </c>
+      <c r="K9">
+        <v>0.101525</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="0"/>
+        <v>1.000092</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10">
+        <v>0.16630524946058092</v>
+      </c>
+      <c r="B10">
+        <v>31114</v>
+      </c>
+      <c r="E10" s="4">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11">
+        <v>0.11946559004149378</v>
+      </c>
+      <c r="B11">
+        <v>31116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12">
+        <v>0.14575827518672199</v>
+      </c>
+      <c r="B12">
+        <v>31296</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13">
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="E14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="4">
+        <v>31104</v>
+      </c>
+      <c r="G14" s="4">
+        <v>31110</v>
+      </c>
+      <c r="H14" s="4">
+        <v>31113</v>
+      </c>
+      <c r="I14" s="4">
+        <v>31114</v>
+      </c>
+      <c r="J14" s="4">
+        <v>31116</v>
+      </c>
+      <c r="K14" s="4">
+        <v>31296</v>
+      </c>
+      <c r="L14" s="4">
+        <v>10000</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="E15" s="4">
+        <v>31104</v>
+      </c>
+      <c r="F15">
+        <f>F4*(1+change31104)</f>
+        <v>8.64624043715847E-2</v>
+      </c>
+      <c r="G15">
+        <f>G4*(1+change31110)</f>
+        <v>0.18902182550335569</v>
+      </c>
+      <c r="H15">
+        <f>H4*(1+change31113)</f>
+        <v>3.3510700636942677E-2</v>
+      </c>
+      <c r="I15">
+        <f>I4*(1+change31114)</f>
+        <v>7.4468431528662407E-2</v>
+      </c>
+      <c r="J15">
+        <v>0.23383100000000001</v>
+      </c>
+      <c r="K15">
+        <v>0.134328</v>
+      </c>
+      <c r="L15">
+        <f>1-O15</f>
+        <v>0.24837763795945456</v>
+      </c>
+      <c r="M15">
+        <f>SUM(F15:L15)</f>
+        <v>1</v>
+      </c>
+      <c r="O15">
+        <v>0.75162236204054544</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="E16" s="4">
+        <v>31110</v>
+      </c>
+      <c r="F16">
+        <f>F5*(1+change31104)</f>
+        <v>0.13791295081967214</v>
+      </c>
+      <c r="G16">
+        <f>G5*(1+change31110)</f>
+        <v>9.9558060402684556E-2</v>
+      </c>
+      <c r="H16">
+        <f>H5*(1+change31113)</f>
+        <v>3.1039832802547768E-2</v>
+      </c>
+      <c r="I16">
+        <f>I5*(1+change31114)</f>
+        <v>0.10001757165605095</v>
+      </c>
+      <c r="J16">
+        <v>0.11981600000000001</v>
+      </c>
+      <c r="K16">
+        <v>0.25345600000000001</v>
+      </c>
+      <c r="L16">
+        <f t="shared" ref="L16:L20" si="1">1-O16</f>
+        <v>0.25819958431904455</v>
+      </c>
+      <c r="M16">
+        <f t="shared" ref="M16:M21" si="2">SUM(F16:L16)</f>
+        <v>1</v>
+      </c>
+      <c r="O16">
+        <v>0.74180041568095545</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="E17" s="4">
+        <v>31113</v>
+      </c>
+      <c r="F17">
+        <f>F6*(1+change31104)</f>
+        <v>6.4667723132969035E-2</v>
+      </c>
+      <c r="G17">
+        <f>G6*(1+change31110)</f>
+        <v>0.23881687248322148</v>
+      </c>
+      <c r="H17">
+        <f>H6*(1+change31113)</f>
+        <v>3.7599251592356685E-2</v>
+      </c>
+      <c r="I17">
+        <f>I6*(1+change31114)</f>
+        <v>5.9084912420382163E-2</v>
+      </c>
+      <c r="J17">
+        <v>0.143541</v>
+      </c>
+      <c r="K17">
+        <v>0.21052599999999999</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="1"/>
+        <v>0.2457642403710707</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O17">
+        <v>0.7542357596289293</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="E18" s="4">
+        <v>31114</v>
+      </c>
+      <c r="F18">
+        <f>F7*(1+change31104)</f>
+        <v>0.19824992714025502</v>
+      </c>
+      <c r="G18">
+        <f>G7*(1+change31110)</f>
+        <v>0.28268794630872485</v>
+      </c>
+      <c r="H18">
+        <f>H7*(1+change31113)</f>
+        <v>1.8376027070063691E-2</v>
+      </c>
+      <c r="I18">
+        <f>I7*(1+change31114)</f>
+        <v>3.8422874203821657E-2</v>
+      </c>
+      <c r="J18">
+        <v>4.4643000000000002E-2</v>
+      </c>
+      <c r="K18">
+        <v>0.21875</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="1"/>
+        <v>0.19887022527713483</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <v>0.80112977472286517</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="E19" s="4">
+        <v>31116</v>
+      </c>
+      <c r="F19">
+        <f>F8*(1+change31104)</f>
+        <v>0.22385887067395266</v>
+      </c>
+      <c r="G19">
+        <f>G8*(1+change31110)</f>
+        <v>0.1781438255033557</v>
+      </c>
+      <c r="H19">
+        <f>H8*(1+change31113)</f>
+        <v>4.0674458598726114E-2</v>
+      </c>
+      <c r="I19">
+        <f>I8*(1+change31114)</f>
+        <v>3.7962603503184707E-2</v>
+      </c>
+      <c r="J19">
+        <v>8.6957000000000007E-2</v>
+      </c>
+      <c r="K19">
+        <v>0.23188400000000001</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="1"/>
+        <v>0.20051924172078084</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O19">
+        <v>0.79948075827921916</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="E20" s="4">
+        <v>31296</v>
+      </c>
+      <c r="F20">
+        <f>F9*(1+change31104)</f>
+        <v>0.11380712204007287</v>
+      </c>
+      <c r="G20">
+        <f>G9*(1+change31110)</f>
+        <v>0.19698402684563757</v>
+      </c>
+      <c r="H20">
+        <f>H9*(1+change31113)</f>
+        <v>7.1494259554140127E-2</v>
+      </c>
+      <c r="I20">
+        <f>I9*(1+change31114)</f>
+        <v>6.997312101910827E-2</v>
+      </c>
+      <c r="J20">
+        <v>0.138211</v>
+      </c>
+      <c r="K20">
+        <v>0.101525</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="1"/>
+        <v>0.30800547054104122</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O20">
+        <v>0.69199452945895878</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="E21" s="4">
+        <v>10000</v>
+      </c>
+      <c r="F21">
+        <f>A7</f>
+        <v>0.15407061712808653</v>
+      </c>
+      <c r="G21">
+        <f>A8</f>
+        <v>0.15090928985602492</v>
+      </c>
+      <c r="H21">
+        <f>A9</f>
+        <v>4.2606034009038771E-2</v>
+      </c>
+      <c r="I21">
+        <f>A10</f>
+        <v>0.16630524946058092</v>
+      </c>
+      <c r="J21">
+        <f>A11</f>
+        <v>0.11946559004149378</v>
+      </c>
+      <c r="K21">
+        <f>A12</f>
+        <v>0.14575827518672199</v>
+      </c>
+      <c r="L21">
+        <f>A6</f>
+        <v>0.22088494431805294</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="F22">
+        <f>SUM(F15:F21)</f>
+        <v>0.97902961530659294</v>
+      </c>
+      <c r="G22">
+        <f t="shared" ref="G22:K22" si="3">SUM(G15:G21)</f>
+        <v>1.3361218469030047</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="3"/>
+        <v>0.27530056426381583</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="3"/>
+        <v>0.54623476379179103</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="3"/>
+        <v>0.88646459004149392</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="3"/>
+        <v>1.2962272751867221</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="B24" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="2">
+        <v>4532</v>
+      </c>
+      <c r="C25" s="2">
+        <v>3975</v>
+      </c>
+      <c r="D25" s="5">
+        <f>(C25-B25)/B25</f>
+        <v>-0.12290379523389232</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="2">
+        <f>SUM(B27:B33)</f>
+        <v>5468</v>
+      </c>
+      <c r="C26" s="2">
+        <f>SUM(C27:C33)</f>
+        <v>6025</v>
+      </c>
+      <c r="D26" s="5">
+        <f t="shared" ref="D26" si="4">(C26-B26)/B26</f>
+        <v>0.10186539868324798</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="1">
+        <v>10000</v>
+      </c>
+      <c r="B27" s="2">
+        <v>0</v>
+      </c>
+      <c r="C27" s="2">
+        <v>1387</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="1">
+        <v>31104</v>
+      </c>
+      <c r="B28" s="2">
+        <v>549</v>
+      </c>
+      <c r="C28" s="2">
+        <v>530</v>
+      </c>
+      <c r="D28" s="5">
+        <f t="shared" ref="D28:D33" si="5">(C28-B28)/B28</f>
+        <v>-3.4608378870673952E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="1">
+        <v>31110</v>
+      </c>
+      <c r="B29" s="2">
+        <v>1639</v>
+      </c>
+      <c r="C29" s="2">
+        <v>1221</v>
+      </c>
+      <c r="D29" s="5">
+        <f t="shared" si="5"/>
+        <v>-0.25503355704697989</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="1">
+        <v>31113</v>
+      </c>
+      <c r="B30" s="2">
+        <v>628</v>
+      </c>
+      <c r="C30" s="2">
+        <v>235</v>
+      </c>
+      <c r="D30" s="5">
+        <f t="shared" si="5"/>
+        <v>-0.62579617834394907</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="1">
+        <v>31114</v>
+      </c>
+      <c r="B31" s="2">
+        <v>189</v>
+      </c>
+      <c r="C31" s="2">
+        <v>189</v>
+      </c>
+      <c r="D31" s="5">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="1">
+        <v>31116</v>
+      </c>
+      <c r="B32" s="2">
+        <v>986</v>
+      </c>
+      <c r="C32" s="2">
+        <v>986</v>
+      </c>
+      <c r="D32" s="5">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="1">
+        <v>31296</v>
+      </c>
+      <c r="B33" s="2">
+        <v>1477</v>
+      </c>
+      <c r="C33" s="2">
+        <v>1477</v>
+      </c>
+      <c r="D33" s="5">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>